<commit_message>
Updated RMI files nov 12-24
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C4">
         <f>EIA!D5</f>
-        <v>-5.3911205073995772E-2</v>
+        <v>-3.382663847780127E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="C5">
         <f>EIA!I5</f>
-        <v>-9.2600248036378743E-2</v>
+        <v>-6.9450186027283992E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="C6">
         <f>EIA!I11</f>
-        <v>-9.4405594405594498E-2</v>
+        <v>-0.11888111888111895</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C9">
         <f>EIA!D3</f>
-        <v>3.9188243526941918E-2</v>
+        <v>3.2890132960111965E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="C11">
         <f>EIA!I3</f>
-        <v>-6.1728395061728371E-2</v>
+        <v>-4.3572984749455312E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C14">
         <f>EIA!D4</f>
-        <v>-6.4206642066420669E-2</v>
+        <v>-5.9778597785977862E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="C16">
         <f>EIA!I4</f>
-        <v>-6.9767441860465129E-2</v>
+        <v>-7.3995771670190377E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1835,13 +1835,13 @@
       </c>
       <c r="C20">
         <f>EIA!C12</f>
-        <v>18168</v>
+        <v>18411</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <f>-(1-C20/B20)</f>
-        <v>-6.5816536404771697E-2</v>
+        <v>-5.3321678321678334E-2</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
@@ -1879,23 +1879,23 @@
       </c>
       <c r="B26" s="6">
         <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-1.2777447982714234E-2</v>
+        <v>-6.4835406216792509E-3</v>
       </c>
       <c r="C26" s="6">
         <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-6.643568474145882E-2</v>
+        <v>-6.5757673833730559E-2</v>
       </c>
       <c r="D26" s="6">
         <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-8.6111701307997141E-2</v>
+        <v>-9.844646725351093E-2</v>
       </c>
       <c r="E26" s="6">
         <f>(EIA!C10-EIA!B10)/EIA!B10</f>
-        <v>-0.12656683305601774</v>
+        <v>-0.13455352190793124</v>
       </c>
       <c r="F26" s="13">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
-        <v>-2.1364221364221364E-2</v>
+        <v>-1.8532818532818532E-2</v>
       </c>
       <c r="G26" s="24"/>
     </row>
@@ -1909,23 +1909,23 @@
       </c>
       <c r="B28" s="11">
         <f>B26/$A$22</f>
-        <v>0.1941373502873644</v>
+        <v>0.12159295854427969</v>
       </c>
       <c r="C28" s="11">
         <f>C26/$A$22</f>
-        <v>1.0094071850405399</v>
+        <v>1.2332258830457008</v>
       </c>
       <c r="D28" s="11">
         <f>D26/$A$22</f>
-        <v>1.3083596617483817</v>
+        <v>1.8462747301314177</v>
       </c>
       <c r="E28" s="11">
         <f>E26/$A$22</f>
-        <v>1.9230248197448696</v>
+        <v>2.5234299846339887</v>
       </c>
       <c r="F28" s="11">
         <f>F26/$A$22</f>
-        <v>0.32460263835263836</v>
+        <v>0.34756630166466224</v>
       </c>
       <c r="G28" s="14"/>
     </row>
@@ -1939,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG181"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AG181"/>
     </sheetView>
   </sheetViews>
@@ -28492,11 +28492,11 @@
         <v>1429</v>
       </c>
       <c r="C3">
-        <v>1485</v>
+        <v>1476</v>
       </c>
       <c r="D3">
         <f>(C3-B3)/B3</f>
-        <v>3.9188243526941918E-2</v>
+        <v>3.2890132960111965E-2</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -28505,11 +28505,11 @@
         <v>13.77</v>
       </c>
       <c r="H3">
-        <v>12.92</v>
+        <v>13.17</v>
       </c>
       <c r="I3">
         <f>(H3-G3)/G3</f>
-        <v>-6.1728395061728371E-2</v>
+        <v>-4.3572984749455312E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -28520,11 +28520,11 @@
         <v>1355</v>
       </c>
       <c r="C4">
-        <v>1268</v>
+        <v>1274</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">(C4-B4)/B4</f>
-        <v>-6.4206642066420669E-2</v>
+        <v>-5.9778597785977862E-2</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -28533,11 +28533,11 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="H4">
-        <v>8.8000000000000007</v>
+        <v>8.76</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I5" si="1">(H4-G4)/G4</f>
-        <v>-6.9767441860465129E-2</v>
+        <v>-7.3995771670190377E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -28548,11 +28548,11 @@
         <v>946</v>
       </c>
       <c r="C5">
-        <v>895</v>
+        <v>914</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-5.3911205073995772E-2</v>
+        <v>-3.382663847780127E-2</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -28561,11 +28561,11 @@
         <v>24.19</v>
       </c>
       <c r="H5">
-        <v>21.95</v>
+        <v>22.51</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-9.2600248036378743E-2</v>
+        <v>-6.9450186027283992E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -28576,11 +28576,11 @@
         <v>3885</v>
       </c>
       <c r="C6">
-        <v>3802</v>
+        <v>3813</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-2.1364221364221364E-2</v>
+        <v>-1.8532818532818532E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -28628,11 +28628,11 @@
         <v>9015</v>
       </c>
       <c r="C10">
-        <v>7874</v>
+        <v>7802</v>
       </c>
       <c r="D10">
         <f>(C10-B10)/B10</f>
-        <v>-0.12656683305601774</v>
+        <v>-0.13455352190793124</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
@@ -28656,11 +28656,11 @@
         <v>28.6</v>
       </c>
       <c r="H11">
-        <v>25.9</v>
+        <v>25.2</v>
       </c>
       <c r="I11">
         <f>(H11-G11)/G11</f>
-        <v>-9.4405594405594498E-2</v>
+        <v>-0.11888111888111895</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -28671,11 +28671,11 @@
         <v>19448</v>
       </c>
       <c r="C12">
-        <v>18168</v>
+        <v>18411</v>
       </c>
       <c r="D12">
         <f>(C12-B12)/B12</f>
-        <v>-6.5816536404771697E-2</v>
+        <v>-5.332167832167832E-2</v>
       </c>
     </row>
   </sheetData>
@@ -28711,7 +28711,7 @@
       </c>
       <c r="B2" s="7">
         <f>Calculations!E28</f>
-        <v>1.9230248197448696</v>
+        <v>2.5234299846339887</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="B3" s="14">
         <f>Calculations!F28</f>
-        <v>0.32460263835263836</v>
+        <v>0.34756630166466224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -28729,7 +28729,7 @@
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.1941373502873644</v>
+        <v>0.12159295854427969</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -28738,7 +28738,7 @@
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>1.0094071850405399</v>
+        <v>1.2332258830457008</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="B6" s="7">
         <f>Calculations!D28</f>
-        <v>1.3083596617483817</v>
+        <v>1.8462747301314177</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>